<commit_message>
Expanded Probe Screening; Updated kcp vs gdd scripts.
</commit_message>
<xml_diff>
--- a/DATA/collate_cultivar_data_new_order/probe_screening/xy_scatter_dfs.xlsx
+++ b/DATA/collate_cultivar_data_new_order/probe_screening/xy_scatter_dfs.xlsx
@@ -11,14 +11,13 @@
     <sheet name="iter_1" sheetId="2" r:id="rId2"/>
     <sheet name="iter_2" sheetId="3" r:id="rId3"/>
     <sheet name="iter_3" sheetId="4" r:id="rId4"/>
-    <sheet name="iter_4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
   <si>
     <t>x_scatter</t>
   </si>
@@ -11454,2030 +11453,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C183"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>0.122449</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>0.1253644</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>0.1146497</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>0.1050955</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>0.1209302</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>7</v>
-      </c>
-      <c r="C7">
-        <v>0.1273585</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>8</v>
-      </c>
-      <c r="C8">
-        <v>0.1170213</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>9</v>
-      </c>
-      <c r="C9">
-        <v>0.0847458</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>17</v>
-      </c>
-      <c r="C10">
-        <v>0.0743494</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>18</v>
-      </c>
-      <c r="C11">
-        <v>0.1046512</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>19</v>
-      </c>
-      <c r="C12">
-        <v>0.1209964</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>20</v>
-      </c>
-      <c r="C13">
-        <v>0.0693069</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>20</v>
-      </c>
-      <c r="C14">
-        <v>0.0990099</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15">
-        <v>22</v>
-      </c>
-      <c r="C15">
-        <v>0.0695187</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>23</v>
-      </c>
-      <c r="C16">
-        <v>0.1107784</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17">
-        <v>23</v>
-      </c>
-      <c r="C17">
-        <v>0.1127451</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18">
-        <v>23</v>
-      </c>
-      <c r="C18">
-        <v>0.0988024</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19">
-        <v>24</v>
-      </c>
-      <c r="C19">
-        <v>0.1190476</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20">
-        <v>25</v>
-      </c>
-      <c r="C20">
-        <v>0.0839695</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21">
-        <v>25</v>
-      </c>
-      <c r="C21">
-        <v>0.0763359</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22">
-        <v>29</v>
-      </c>
-      <c r="C22">
-        <v>0.1030303</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23">
-        <v>30</v>
-      </c>
-      <c r="C23">
-        <v>0.0993521</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="B24">
-        <v>30</v>
-      </c>
-      <c r="C24">
-        <v>0.1187905</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="B25">
-        <v>32</v>
-      </c>
-      <c r="C25">
-        <v>0.1420455</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="1">
-        <v>24</v>
-      </c>
-      <c r="B26">
-        <v>32</v>
-      </c>
-      <c r="C26">
-        <v>0.08522730000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="1">
-        <v>25</v>
-      </c>
-      <c r="B27">
-        <v>33</v>
-      </c>
-      <c r="C27">
-        <v>0.1437908</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="1">
-        <v>26</v>
-      </c>
-      <c r="B28">
-        <v>33</v>
-      </c>
-      <c r="C28">
-        <v>0.09230770000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="1">
-        <v>27</v>
-      </c>
-      <c r="B29">
-        <v>34</v>
-      </c>
-      <c r="C29">
-        <v>0.1472868</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="1">
-        <v>28</v>
-      </c>
-      <c r="B30">
-        <v>34</v>
-      </c>
-      <c r="C30">
-        <v>0.124031</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="1">
-        <v>29</v>
-      </c>
-      <c r="B31">
-        <v>34</v>
-      </c>
-      <c r="C31">
-        <v>0.1384615</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="1">
-        <v>30</v>
-      </c>
-      <c r="B32">
-        <v>35</v>
-      </c>
-      <c r="C32">
-        <v>0.1088083</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="1">
-        <v>31</v>
-      </c>
-      <c r="B33">
-        <v>35</v>
-      </c>
-      <c r="C33">
-        <v>0.1243523</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="1">
-        <v>32</v>
-      </c>
-      <c r="B34">
-        <v>36</v>
-      </c>
-      <c r="C34">
-        <v>0.127551</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="1">
-        <v>33</v>
-      </c>
-      <c r="B35">
-        <v>37</v>
-      </c>
-      <c r="C35">
-        <v>0.107438</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="1">
-        <v>34</v>
-      </c>
-      <c r="B36">
-        <v>37</v>
-      </c>
-      <c r="C36">
-        <v>0.1487603</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="1">
-        <v>35</v>
-      </c>
-      <c r="B37">
-        <v>38</v>
-      </c>
-      <c r="C37">
-        <v>0.1172161</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="1">
-        <v>36</v>
-      </c>
-      <c r="B38">
-        <v>38</v>
-      </c>
-      <c r="C38">
-        <v>0.09157510000000001</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="1">
-        <v>37</v>
-      </c>
-      <c r="B39">
-        <v>40</v>
-      </c>
-      <c r="C39">
-        <v>0.1348315</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="1">
-        <v>38</v>
-      </c>
-      <c r="B40">
-        <v>41</v>
-      </c>
-      <c r="C40">
-        <v>0.1542289</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="1">
-        <v>39</v>
-      </c>
-      <c r="B41">
-        <v>42</v>
-      </c>
-      <c r="C41">
-        <v>0.102439</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="1">
-        <v>40</v>
-      </c>
-      <c r="B42">
-        <v>44</v>
-      </c>
-      <c r="C42">
-        <v>0.1259259</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="1">
-        <v>41</v>
-      </c>
-      <c r="B43">
-        <v>49</v>
-      </c>
-      <c r="C43">
-        <v>0.145749</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="1">
-        <v>42</v>
-      </c>
-      <c r="B44">
-        <v>49</v>
-      </c>
-      <c r="C44">
-        <v>0.1318052</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="1">
-        <v>43</v>
-      </c>
-      <c r="B45">
-        <v>51</v>
-      </c>
-      <c r="C45">
-        <v>0.1502347</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="1">
-        <v>44</v>
-      </c>
-      <c r="B46">
-        <v>53</v>
-      </c>
-      <c r="C46">
-        <v>0.1280488</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="1">
-        <v>45</v>
-      </c>
-      <c r="B47">
-        <v>53</v>
-      </c>
-      <c r="C47">
-        <v>0.1158537</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="1">
-        <v>46</v>
-      </c>
-      <c r="B48">
-        <v>54</v>
-      </c>
-      <c r="C48">
-        <v>0.095679</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="1">
-        <v>47</v>
-      </c>
-      <c r="B49">
-        <v>54</v>
-      </c>
-      <c r="C49">
-        <v>0.1022727</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="1">
-        <v>48</v>
-      </c>
-      <c r="B50">
-        <v>57</v>
-      </c>
-      <c r="C50">
-        <v>0.1198157</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="1">
-        <v>49</v>
-      </c>
-      <c r="B51">
-        <v>58</v>
-      </c>
-      <c r="C51">
-        <v>0.1486811</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="1">
-        <v>50</v>
-      </c>
-      <c r="B52">
-        <v>62</v>
-      </c>
-      <c r="C52">
-        <v>0.1176471</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="1">
-        <v>51</v>
-      </c>
-      <c r="B53">
-        <v>62</v>
-      </c>
-      <c r="C53">
-        <v>0.1232493</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="1">
-        <v>52</v>
-      </c>
-      <c r="B54">
-        <v>62</v>
-      </c>
-      <c r="C54">
-        <v>0.1192308</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="1">
-        <v>53</v>
-      </c>
-      <c r="B55">
-        <v>63</v>
-      </c>
-      <c r="C55">
-        <v>0.0943396</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="1">
-        <v>54</v>
-      </c>
-      <c r="B56">
-        <v>63</v>
-      </c>
-      <c r="C56">
-        <v>0.0825472</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="1">
-        <v>55</v>
-      </c>
-      <c r="B57">
-        <v>64</v>
-      </c>
-      <c r="C57">
-        <v>0.07142859999999999</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="1">
-        <v>56</v>
-      </c>
-      <c r="B58">
-        <v>69</v>
-      </c>
-      <c r="C58">
-        <v>0.07853400000000001</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="1">
-        <v>57</v>
-      </c>
-      <c r="B59">
-        <v>70</v>
-      </c>
-      <c r="C59">
-        <v>0.1138015</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="1">
-        <v>58</v>
-      </c>
-      <c r="B60">
-        <v>71</v>
-      </c>
-      <c r="C60">
-        <v>0.1021021</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="1">
-        <v>59</v>
-      </c>
-      <c r="B61">
-        <v>72</v>
-      </c>
-      <c r="C61">
-        <v>0.0826446</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="1">
-        <v>60</v>
-      </c>
-      <c r="B62">
-        <v>72</v>
-      </c>
-      <c r="C62">
-        <v>0.0751445</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="1">
-        <v>61</v>
-      </c>
-      <c r="B63">
-        <v>75</v>
-      </c>
-      <c r="C63">
-        <v>0.09230770000000001</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="1">
-        <v>62</v>
-      </c>
-      <c r="B64">
-        <v>75</v>
-      </c>
-      <c r="C64">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="1">
-        <v>63</v>
-      </c>
-      <c r="B65">
-        <v>76</v>
-      </c>
-      <c r="C65">
-        <v>0.0786517</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="1">
-        <v>64</v>
-      </c>
-      <c r="B66">
-        <v>76</v>
-      </c>
-      <c r="C66">
-        <v>0.1155378</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="1">
-        <v>65</v>
-      </c>
-      <c r="B67">
-        <v>77</v>
-      </c>
-      <c r="C67">
-        <v>0.0932945</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="1">
-        <v>66</v>
-      </c>
-      <c r="B68">
-        <v>78</v>
-      </c>
-      <c r="C68">
-        <v>0.09843399999999999</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="1">
-        <v>67</v>
-      </c>
-      <c r="B69">
-        <v>80</v>
-      </c>
-      <c r="C69">
-        <v>0.08398949999999999</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="1">
-        <v>68</v>
-      </c>
-      <c r="B70">
-        <v>81</v>
-      </c>
-      <c r="C70">
-        <v>0.1011673</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="1">
-        <v>69</v>
-      </c>
-      <c r="B71">
-        <v>83</v>
-      </c>
-      <c r="C71">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="1">
-        <v>70</v>
-      </c>
-      <c r="B72">
-        <v>83</v>
-      </c>
-      <c r="C72">
-        <v>0.094697</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="1">
-        <v>71</v>
-      </c>
-      <c r="B73">
-        <v>84</v>
-      </c>
-      <c r="C73">
-        <v>0.0705128</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="1">
-        <v>72</v>
-      </c>
-      <c r="B74">
-        <v>84</v>
-      </c>
-      <c r="C74">
-        <v>0.08883249999999999</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="1">
-        <v>73</v>
-      </c>
-      <c r="B75">
-        <v>84</v>
-      </c>
-      <c r="C75">
-        <v>0.08119659999999999</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="1">
-        <v>74</v>
-      </c>
-      <c r="B76">
-        <v>85</v>
-      </c>
-      <c r="C76">
-        <v>0.0841837</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="1">
-        <v>75</v>
-      </c>
-      <c r="B77">
-        <v>85</v>
-      </c>
-      <c r="C77">
-        <v>0.0841837</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" s="1">
-        <v>76</v>
-      </c>
-      <c r="B78">
-        <v>89</v>
-      </c>
-      <c r="C78">
-        <v>0.07383969999999999</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="1">
-        <v>77</v>
-      </c>
-      <c r="B79">
-        <v>90</v>
-      </c>
-      <c r="C79">
-        <v>0.0835735</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="1">
-        <v>78</v>
-      </c>
-      <c r="B80">
-        <v>90</v>
-      </c>
-      <c r="C80">
-        <v>0.1066282</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="1">
-        <v>79</v>
-      </c>
-      <c r="B81">
-        <v>90</v>
-      </c>
-      <c r="C81">
-        <v>0.08461539999999999</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="1">
-        <v>80</v>
-      </c>
-      <c r="B82">
-        <v>91</v>
-      </c>
-      <c r="C82">
-        <v>0.09090910000000001</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="1">
-        <v>81</v>
-      </c>
-      <c r="B83">
-        <v>91</v>
-      </c>
-      <c r="C83">
-        <v>0.08053689999999999</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" s="1">
-        <v>82</v>
-      </c>
-      <c r="B84">
-        <v>93</v>
-      </c>
-      <c r="C84">
-        <v>0.1332149</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" s="1">
-        <v>83</v>
-      </c>
-      <c r="B85">
-        <v>95</v>
-      </c>
-      <c r="C85">
-        <v>0.1945525</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" s="1">
-        <v>84</v>
-      </c>
-      <c r="B86">
-        <v>96</v>
-      </c>
-      <c r="C86">
-        <v>0.1259542</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" s="1">
-        <v>85</v>
-      </c>
-      <c r="B87">
-        <v>97</v>
-      </c>
-      <c r="C87">
-        <v>0.1254545</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" s="1">
-        <v>86</v>
-      </c>
-      <c r="B88">
-        <v>98</v>
-      </c>
-      <c r="C88">
-        <v>0.1403813</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89" s="1">
-        <v>87</v>
-      </c>
-      <c r="B89">
-        <v>101</v>
-      </c>
-      <c r="C89">
-        <v>0.1855422</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" s="1">
-        <v>88</v>
-      </c>
-      <c r="B90">
-        <v>103</v>
-      </c>
-      <c r="C90">
-        <v>0.1637168</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" s="1">
-        <v>89</v>
-      </c>
-      <c r="B91">
-        <v>104</v>
-      </c>
-      <c r="C91">
-        <v>0.1709559</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="A92" s="1">
-        <v>90</v>
-      </c>
-      <c r="B92">
-        <v>104</v>
-      </c>
-      <c r="C92">
-        <v>0.1943888</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="A93" s="1">
-        <v>91</v>
-      </c>
-      <c r="B93">
-        <v>119</v>
-      </c>
-      <c r="C93">
-        <v>0.1872279</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="A94" s="1">
-        <v>92</v>
-      </c>
-      <c r="B94">
-        <v>119</v>
-      </c>
-      <c r="C94">
-        <v>0.1393324</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
-      <c r="A95" s="1">
-        <v>93</v>
-      </c>
-      <c r="B95">
-        <v>120</v>
-      </c>
-      <c r="C95">
-        <v>0.1767372</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3">
-      <c r="A96" s="1">
-        <v>94</v>
-      </c>
-      <c r="B96">
-        <v>121</v>
-      </c>
-      <c r="C96">
-        <v>0.1458626</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
-      <c r="A97" s="1">
-        <v>95</v>
-      </c>
-      <c r="B97">
-        <v>123</v>
-      </c>
-      <c r="C97">
-        <v>0.2715827</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
-      <c r="A98" s="1">
-        <v>96</v>
-      </c>
-      <c r="B98">
-        <v>125</v>
-      </c>
-      <c r="C98">
-        <v>0.3282548</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
-      <c r="A99" s="1">
-        <v>97</v>
-      </c>
-      <c r="B99">
-        <v>128</v>
-      </c>
-      <c r="C99">
-        <v>0.3890411</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
-      <c r="A100" s="1">
-        <v>98</v>
-      </c>
-      <c r="B100">
-        <v>131</v>
-      </c>
-      <c r="C100">
-        <v>0.2710997</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3">
-      <c r="A101" s="1">
-        <v>99</v>
-      </c>
-      <c r="B101">
-        <v>133</v>
-      </c>
-      <c r="C101">
-        <v>0.3011152</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
-      <c r="A102" s="1">
-        <v>100</v>
-      </c>
-      <c r="B102">
-        <v>136</v>
-      </c>
-      <c r="C102">
-        <v>0.2340426</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
-      <c r="A103" s="1">
-        <v>101</v>
-      </c>
-      <c r="B103">
-        <v>145</v>
-      </c>
-      <c r="C103">
-        <v>0.3317647</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
-      <c r="A104" s="1">
-        <v>102</v>
-      </c>
-      <c r="B104">
-        <v>146</v>
-      </c>
-      <c r="C104">
-        <v>0.3663194</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3">
-      <c r="A105" s="1">
-        <v>103</v>
-      </c>
-      <c r="B105">
-        <v>149</v>
-      </c>
-      <c r="C105">
-        <v>0.2176235</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
-      <c r="A106" s="1">
-        <v>104</v>
-      </c>
-      <c r="B106">
-        <v>150</v>
-      </c>
-      <c r="C106">
-        <v>0.223565</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="A107" s="1">
-        <v>105</v>
-      </c>
-      <c r="B107">
-        <v>156</v>
-      </c>
-      <c r="C107">
-        <v>0.4278075</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
-      <c r="A108" s="1">
-        <v>106</v>
-      </c>
-      <c r="B108">
-        <v>156</v>
-      </c>
-      <c r="C108">
-        <v>0.5288462</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3">
-      <c r="A109" s="1">
-        <v>107</v>
-      </c>
-      <c r="B109">
-        <v>156</v>
-      </c>
-      <c r="C109">
-        <v>0.315197</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3">
-      <c r="A110" s="1">
-        <v>108</v>
-      </c>
-      <c r="B110">
-        <v>157</v>
-      </c>
-      <c r="C110">
-        <v>0.2943662</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3">
-      <c r="A111" s="1">
-        <v>109</v>
-      </c>
-      <c r="B111">
-        <v>171</v>
-      </c>
-      <c r="C111">
-        <v>0.2971429</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3">
-      <c r="A112" s="1">
-        <v>110</v>
-      </c>
-      <c r="B112">
-        <v>171</v>
-      </c>
-      <c r="C112">
-        <v>0.4149933</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3">
-      <c r="A113" s="1">
-        <v>111</v>
-      </c>
-      <c r="B113">
-        <v>173</v>
-      </c>
-      <c r="C113">
-        <v>0.5082873</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3">
-      <c r="A114" s="1">
-        <v>112</v>
-      </c>
-      <c r="B114">
-        <v>176</v>
-      </c>
-      <c r="C114">
-        <v>0.3267717</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3">
-      <c r="A115" s="1">
-        <v>113</v>
-      </c>
-      <c r="B115">
-        <v>178</v>
-      </c>
-      <c r="C115">
-        <v>0.3736264</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3">
-      <c r="A116" s="1">
-        <v>114</v>
-      </c>
-      <c r="B116">
-        <v>179</v>
-      </c>
-      <c r="C116">
-        <v>0.3533026</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3">
-      <c r="A117" s="1">
-        <v>115</v>
-      </c>
-      <c r="B117">
-        <v>179</v>
-      </c>
-      <c r="C117">
-        <v>0.3839662</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3">
-      <c r="A118" s="1">
-        <v>116</v>
-      </c>
-      <c r="B118">
-        <v>181</v>
-      </c>
-      <c r="C118">
-        <v>0.3410138</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3">
-      <c r="A119" s="1">
-        <v>117</v>
-      </c>
-      <c r="B119">
-        <v>182</v>
-      </c>
-      <c r="C119">
-        <v>0.2560241</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
-      <c r="A120" s="1">
-        <v>118</v>
-      </c>
-      <c r="B120">
-        <v>187</v>
-      </c>
-      <c r="C120">
-        <v>0.5576923</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3">
-      <c r="A121" s="1">
-        <v>119</v>
-      </c>
-      <c r="B121">
-        <v>187</v>
-      </c>
-      <c r="C121">
-        <v>0.4344392</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3">
-      <c r="A122" s="1">
-        <v>120</v>
-      </c>
-      <c r="B122">
-        <v>192</v>
-      </c>
-      <c r="C122">
-        <v>0.4695122</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3">
-      <c r="A123" s="1">
-        <v>121</v>
-      </c>
-      <c r="B123">
-        <v>197</v>
-      </c>
-      <c r="C123">
-        <v>0.6212361</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3">
-      <c r="A124" s="1">
-        <v>122</v>
-      </c>
-      <c r="B124">
-        <v>197</v>
-      </c>
-      <c r="C124">
-        <v>0.3317972</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3">
-      <c r="A125" s="1">
-        <v>123</v>
-      </c>
-      <c r="B125">
-        <v>197</v>
-      </c>
-      <c r="C125">
-        <v>0.451664</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3">
-      <c r="A126" s="1">
-        <v>124</v>
-      </c>
-      <c r="B126">
-        <v>198</v>
-      </c>
-      <c r="C126">
-        <v>0.4154676</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3">
-      <c r="A127" s="1">
-        <v>125</v>
-      </c>
-      <c r="B127">
-        <v>199</v>
-      </c>
-      <c r="C127">
-        <v>0.5191041</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3">
-      <c r="A128" s="1">
-        <v>126</v>
-      </c>
-      <c r="B128">
-        <v>201</v>
-      </c>
-      <c r="C128">
-        <v>0.6185853</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3">
-      <c r="A129" s="1">
-        <v>127</v>
-      </c>
-      <c r="B129">
-        <v>203</v>
-      </c>
-      <c r="C129">
-        <v>0.5660036000000001</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3">
-      <c r="A130" s="1">
-        <v>128</v>
-      </c>
-      <c r="B130">
-        <v>204</v>
-      </c>
-      <c r="C130">
-        <v>0.3660856</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3">
-      <c r="A131" s="1">
-        <v>129</v>
-      </c>
-      <c r="B131">
-        <v>206</v>
-      </c>
-      <c r="C131">
-        <v>0.4397993</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3">
-      <c r="A132" s="1">
-        <v>130</v>
-      </c>
-      <c r="B132">
-        <v>209</v>
-      </c>
-      <c r="C132">
-        <v>0.5483871</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3">
-      <c r="A133" s="1">
-        <v>131</v>
-      </c>
-      <c r="B133">
-        <v>210</v>
-      </c>
-      <c r="C133">
-        <v>0.3723776</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3">
-      <c r="A134" s="1">
-        <v>132</v>
-      </c>
-      <c r="B134">
-        <v>211</v>
-      </c>
-      <c r="C134">
-        <v>0.4456522</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3">
-      <c r="A135" s="1">
-        <v>133</v>
-      </c>
-      <c r="B135">
-        <v>213</v>
-      </c>
-      <c r="C135">
-        <v>0.535316</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3">
-      <c r="A136" s="1">
-        <v>134</v>
-      </c>
-      <c r="B136">
-        <v>214</v>
-      </c>
-      <c r="C136">
-        <v>0.3900344</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3">
-      <c r="A137" s="1">
-        <v>135</v>
-      </c>
-      <c r="B137">
-        <v>215</v>
-      </c>
-      <c r="C137">
-        <v>0.3333333</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3">
-      <c r="A138" s="1">
-        <v>136</v>
-      </c>
-      <c r="B138">
-        <v>217</v>
-      </c>
-      <c r="C138">
-        <v>0.3359746</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3">
-      <c r="A139" s="1">
-        <v>137</v>
-      </c>
-      <c r="B139">
-        <v>219</v>
-      </c>
-      <c r="C139">
-        <v>0.4263658</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3">
-      <c r="A140" s="1">
-        <v>138</v>
-      </c>
-      <c r="B140">
-        <v>220</v>
-      </c>
-      <c r="C140">
-        <v>0.4227941</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3">
-      <c r="A141" s="1">
-        <v>139</v>
-      </c>
-      <c r="B141">
-        <v>220</v>
-      </c>
-      <c r="C141">
-        <v>0.5514706</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3">
-      <c r="A142" s="1">
-        <v>140</v>
-      </c>
-      <c r="B142">
-        <v>220</v>
-      </c>
-      <c r="C142">
-        <v>0.5022971000000001</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3">
-      <c r="A143" s="1">
-        <v>141</v>
-      </c>
-      <c r="B143">
-        <v>221</v>
-      </c>
-      <c r="C143">
-        <v>0.4769688</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3">
-      <c r="A144" s="1">
-        <v>142</v>
-      </c>
-      <c r="B144">
-        <v>228</v>
-      </c>
-      <c r="C144">
-        <v>0.6065891</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3">
-      <c r="A145" s="1">
-        <v>143</v>
-      </c>
-      <c r="B145">
-        <v>229</v>
-      </c>
-      <c r="C145">
-        <v>0.6424051</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3">
-      <c r="A146" s="1">
-        <v>144</v>
-      </c>
-      <c r="B146">
-        <v>230</v>
-      </c>
-      <c r="C146">
-        <v>0.3713235</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3">
-      <c r="A147" s="1">
-        <v>145</v>
-      </c>
-      <c r="B147">
-        <v>232</v>
-      </c>
-      <c r="C147">
-        <v>0.3625</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3">
-      <c r="A148" s="1">
-        <v>146</v>
-      </c>
-      <c r="B148">
-        <v>232</v>
-      </c>
-      <c r="C148">
-        <v>0.4791667</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3">
-      <c r="A149" s="1">
-        <v>147</v>
-      </c>
-      <c r="B149">
-        <v>234</v>
-      </c>
-      <c r="C149">
-        <v>0.585736</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3">
-      <c r="A150" s="1">
-        <v>148</v>
-      </c>
-      <c r="B150">
-        <v>234</v>
-      </c>
-      <c r="C150">
-        <v>0.5538695</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3">
-      <c r="A151" s="1">
-        <v>149</v>
-      </c>
-      <c r="B151">
-        <v>235</v>
-      </c>
-      <c r="C151">
-        <v>0.4393305</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3">
-      <c r="A152" s="1">
-        <v>150</v>
-      </c>
-      <c r="B152">
-        <v>241</v>
-      </c>
-      <c r="C152">
-        <v>0.4030303</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3">
-      <c r="A153" s="1">
-        <v>151</v>
-      </c>
-      <c r="B153">
-        <v>242</v>
-      </c>
-      <c r="C153">
-        <v>0.43898</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3">
-      <c r="A154" s="1">
-        <v>152</v>
-      </c>
-      <c r="B154">
-        <v>247</v>
-      </c>
-      <c r="C154">
-        <v>0.3944954</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3">
-      <c r="A155" s="1">
-        <v>153</v>
-      </c>
-      <c r="B155">
-        <v>249</v>
-      </c>
-      <c r="C155">
-        <v>0.6469003</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3">
-      <c r="A156" s="1">
-        <v>154</v>
-      </c>
-      <c r="B156">
-        <v>251</v>
-      </c>
-      <c r="C156">
-        <v>0.5582734</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3">
-      <c r="A157" s="1">
-        <v>155</v>
-      </c>
-      <c r="B157">
-        <v>255</v>
-      </c>
-      <c r="C157">
-        <v>0.2525773</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3">
-      <c r="A158" s="1">
-        <v>156</v>
-      </c>
-      <c r="B158">
-        <v>258</v>
-      </c>
-      <c r="C158">
-        <v>0.403397</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3">
-      <c r="A159" s="1">
-        <v>157</v>
-      </c>
-      <c r="B159">
-        <v>259</v>
-      </c>
-      <c r="C159">
-        <v>0.4233871</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3">
-      <c r="A160" s="1">
-        <v>158</v>
-      </c>
-      <c r="B160">
-        <v>260</v>
-      </c>
-      <c r="C160">
-        <v>0.4324324</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3">
-      <c r="A161" s="1">
-        <v>159</v>
-      </c>
-      <c r="B161">
-        <v>261</v>
-      </c>
-      <c r="C161">
-        <v>0.3315927</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3">
-      <c r="A162" s="1">
-        <v>160</v>
-      </c>
-      <c r="B162">
-        <v>262</v>
-      </c>
-      <c r="C162">
-        <v>0.3502415</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3">
-      <c r="A163" s="1">
-        <v>161</v>
-      </c>
-      <c r="B163">
-        <v>263</v>
-      </c>
-      <c r="C163">
-        <v>0.4752137</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3">
-      <c r="A164" s="1">
-        <v>162</v>
-      </c>
-      <c r="B164">
-        <v>266</v>
-      </c>
-      <c r="C164">
-        <v>0.2880658</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3">
-      <c r="A165" s="1">
-        <v>163</v>
-      </c>
-      <c r="B165">
-        <v>272</v>
-      </c>
-      <c r="C165">
-        <v>0.4217252</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3">
-      <c r="A166" s="1">
-        <v>164</v>
-      </c>
-      <c r="B166">
-        <v>272</v>
-      </c>
-      <c r="C166">
-        <v>0.3628692</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3">
-      <c r="A167" s="1">
-        <v>165</v>
-      </c>
-      <c r="B167">
-        <v>275</v>
-      </c>
-      <c r="C167">
-        <v>0.4662757</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3">
-      <c r="A168" s="1">
-        <v>166</v>
-      </c>
-      <c r="B168">
-        <v>276</v>
-      </c>
-      <c r="C168">
-        <v>0.3198198</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3">
-      <c r="A169" s="1">
-        <v>167</v>
-      </c>
-      <c r="B169">
-        <v>284</v>
-      </c>
-      <c r="C169">
-        <v>0.2924791</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3">
-      <c r="A170" s="1">
-        <v>168</v>
-      </c>
-      <c r="B170">
-        <v>284</v>
-      </c>
-      <c r="C170">
-        <v>0.2928571</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3">
-      <c r="A171" s="1">
-        <v>169</v>
-      </c>
-      <c r="B171">
-        <v>288</v>
-      </c>
-      <c r="C171">
-        <v>0.2696897</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3">
-      <c r="A172" s="1">
-        <v>170</v>
-      </c>
-      <c r="B172">
-        <v>289</v>
-      </c>
-      <c r="C172">
-        <v>0.5033408</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3">
-      <c r="A173" s="1">
-        <v>171</v>
-      </c>
-      <c r="B173">
-        <v>298</v>
-      </c>
-      <c r="C173">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3">
-      <c r="A174" s="1">
-        <v>172</v>
-      </c>
-      <c r="B174">
-        <v>299</v>
-      </c>
-      <c r="C174">
-        <v>0.3418079</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3">
-      <c r="A175" s="1">
-        <v>173</v>
-      </c>
-      <c r="B175">
-        <v>307</v>
-      </c>
-      <c r="C175">
-        <v>0.2011494</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3">
-      <c r="A176" s="1">
-        <v>174</v>
-      </c>
-      <c r="B176">
-        <v>308</v>
-      </c>
-      <c r="C176">
-        <v>0.1826625</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3">
-      <c r="A177" s="1">
-        <v>175</v>
-      </c>
-      <c r="B177">
-        <v>309</v>
-      </c>
-      <c r="C177">
-        <v>0.1657609</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3">
-      <c r="A178" s="1">
-        <v>176</v>
-      </c>
-      <c r="B178">
-        <v>311</v>
-      </c>
-      <c r="C178">
-        <v>0.2068966</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3">
-      <c r="A179" s="1">
-        <v>177</v>
-      </c>
-      <c r="B179">
-        <v>315</v>
-      </c>
-      <c r="C179">
-        <v>0.2135417</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3">
-      <c r="A180" s="1">
-        <v>178</v>
-      </c>
-      <c r="B180">
-        <v>316</v>
-      </c>
-      <c r="C180">
-        <v>0.2086168</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3">
-      <c r="A181" s="1">
-        <v>179</v>
-      </c>
-      <c r="B181">
-        <v>317</v>
-      </c>
-      <c r="C181">
-        <v>0.1458333</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3">
-      <c r="A182" s="1">
-        <v>180</v>
-      </c>
-      <c r="B182">
-        <v>344</v>
-      </c>
-      <c r="C182">
-        <v>0.0943396</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3">
-      <c r="A183" s="1">
-        <v>181</v>
-      </c>
-      <c r="B183">
-        <v>348</v>
-      </c>
-      <c r="C183">
-        <v>0.1046512</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>